<commit_message>
TC0031 TC0032 refractored to use data provider for more stable test and included IIR verifications in summary page
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontariogov-my.sharepoint.com/personal/mark_belleza_ontario_ca/Documents/code backup/SeleniumTest/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{5FE7C642-125E-4A8A-BB37-B6306D387514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1785ED4A-1C24-4A66-B424-5AC4EE4DEDC0}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{5FE7C642-125E-4A8A-BB37-B6306D387514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D008FEC7-5667-49CC-AE0E-0B3677F33660}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{AED11CA9-1F75-46C2-A348-8D07D0C95F51}"/>
+    <workbookView xWindow="6630" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{AED11CA9-1F75-46C2-A348-8D07D0C95F51}"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" r:id="rId1"/>
     <sheet name="Regional Office Locations" sheetId="2" r:id="rId2"/>
+    <sheet name="Department1" sheetId="3" r:id="rId3"/>
+    <sheet name="Department3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>THUNDER BAY JAIL - ADULT</t>
   </si>
@@ -127,6 +129,33 @@
   </si>
   <si>
     <t>Western Regional Office</t>
+  </si>
+  <si>
+    <t>Correctional Services Oversight &amp; Investigations</t>
+  </si>
+  <si>
+    <t>Family Liaison Support</t>
+  </si>
+  <si>
+    <t>Institution Admin Support</t>
+  </si>
+  <si>
+    <t>Operational Support Division</t>
+  </si>
+  <si>
+    <t>Safer Team</t>
+  </si>
+  <si>
+    <t>Statistical Analysis Unit</t>
+  </si>
+  <si>
+    <t>ADM Office of the Institutional Services</t>
+  </si>
+  <si>
+    <t>Executive Directors Office</t>
+  </si>
+  <si>
+    <t>Information Management Unit</t>
   </si>
 </sst>
 </file>
@@ -620,7 +649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF616288-EC4F-4246-83CE-146894A05974}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -655,6 +684,81 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE30F238-E6A7-4701-8BAE-7920FC6CC6F3}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A407D11-792A-4C82-8C27-66C47C71E439}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{034a106e-6316-442c-ad35-738afd673d2b}" enabled="1" method="Standard" siteId="{cddc1229-ac2a-4b97-b78a-0e5cacb5865c}" removed="0"/>

</xml_diff>